<commit_message>
Add debug prints to create_orders and add resource_tree_transfer method
</commit_message>
<xml_diff>
--- a/unilabos/devices/workstation/bioyond_studio/bioyond_cell/2025092701.xlsx
+++ b/unilabos/devices/workstation/bioyond_studio/bioyond_cell/2025092701.xlsx
@@ -502,10 +502,10 @@
         <v>配液小瓶</v>
       </c>
       <c r="E2" t="str">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="F2" t="str">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="H2" t="str">
         <v>0</v>
@@ -514,13 +514,13 @@
         <v>0</v>
       </c>
       <c r="J2" t="str">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K2" t="str">
         <v>0</v>
       </c>
       <c r="N2" t="str">
-        <v>0.1</v>
+        <v/>
       </c>
       <c r="O2" t="str">
         <v>0</v>
@@ -579,15 +579,15 @@
         <v>配液小瓶</v>
       </c>
       <c r="E3" t="str">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="F3" t="str">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="H3" t="str">
         <v>0</v>
       </c>
-      <c r="N3" t="str">
+      <c r="J3" t="str">
         <v>0.15</v>
       </c>
       <c r="AA3" t="str">

</xml_diff>

<commit_message>
Update YB resources: add YB_ prefix to models and update deck configurations
</commit_message>
<xml_diff>
--- a/unilabos/devices/workstation/bioyond_studio/bioyond_cell/2025092701.xlsx
+++ b/unilabos/devices/workstation/bioyond_studio/bioyond_cell/2025092701.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -502,7 +502,7 @@
         <v>配液小瓶</v>
       </c>
       <c r="E2" t="str">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F2" t="str">
         <v>0.1</v>
@@ -553,50 +553,21 @@
         <v>0</v>
       </c>
       <c r="Y2" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z2" t="str">
         <v>0</v>
       </c>
       <c r="AA2" t="str">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AB2" t="str">
         <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>TEST-02</v>
-      </c>
-      <c r="B3" t="str">
-        <v>DP20250927002</v>
-      </c>
-      <c r="C3" t="str">
-        <v>9/27/25</v>
-      </c>
-      <c r="D3" t="str">
-        <v>配液小瓶</v>
-      </c>
-      <c r="E3" t="str">
-        <v>30</v>
-      </c>
-      <c r="F3" t="str">
-        <v>0.1</v>
-      </c>
-      <c r="H3" t="str">
-        <v>0</v>
-      </c>
-      <c r="J3" t="str">
-        <v>0.15</v>
-      </c>
-      <c r="AA3" t="str">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AB3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AB2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: 更新 Excel 模板文件
- 更新 2025092701.xlsx 配方文件
- 更新 material_template.xlsx 物料模板
</commit_message>
<xml_diff>
--- a/unilabos/devices/workstation/bioyond_studio/bioyond_cell/2025092701.xlsx
+++ b/unilabos/devices/workstation/bioyond_studio/bioyond_cell/2025092701.xlsx
@@ -1,50 +1,187 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\67484\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1BA2BF-7760-496B-8B47-D20B84F44276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-8070" yWindow="880" windowWidth="17570" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="场景1 完成扣电and电导配液，以及部分单独软包配液" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+  <si>
+    <t>算法批次</t>
+  </si>
+  <si>
+    <t>配方ID</t>
+  </si>
+  <si>
+    <t>创建日期</t>
+  </si>
+  <si>
+    <t>配液瓶类型</t>
+  </si>
+  <si>
+    <t>混匀时间(s)</t>
+  </si>
+  <si>
+    <t>扣电组装分液体积</t>
+  </si>
+  <si>
+    <t>软包组装分液体积</t>
+  </si>
+  <si>
+    <t>电导测试分液体积</t>
+  </si>
+  <si>
+    <t>电导测试分液瓶数</t>
+  </si>
+  <si>
+    <t>LiPF6(g)</t>
+  </si>
+  <si>
+    <t>LiDFOB(g)</t>
+  </si>
+  <si>
+    <t>DTD(g)</t>
+  </si>
+  <si>
+    <t>SA(g)</t>
+  </si>
+  <si>
+    <t>LiPO2F2(g)</t>
+  </si>
+  <si>
+    <t>TEST-02</t>
+  </si>
+  <si>
+    <t>DP20250927001</t>
+  </si>
+  <si>
+    <t>9/27/25</t>
+  </si>
+  <si>
+    <t>配液小瓶</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>LiFSI(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LiTFSI(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LiNO3(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMC(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMC(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VC(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADN(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTCN(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DENE(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TMSP(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEC(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SN(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F2EA(g)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -68,14 +205,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -400,172 +546,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="9.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>算法批次</v>
-      </c>
-      <c r="B1" t="str">
-        <v>配方ID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>创建日期</v>
-      </c>
-      <c r="D1" t="str">
-        <v>配液瓶类型</v>
-      </c>
-      <c r="E1" t="str">
-        <v>混匀时间(s)</v>
-      </c>
-      <c r="F1" t="str">
-        <v>扣电组装分液体积</v>
-      </c>
-      <c r="G1" t="str">
-        <v>软包组装分液体积</v>
-      </c>
-      <c r="H1" t="str">
-        <v>电导测试分液体积</v>
-      </c>
-      <c r="I1" t="str">
-        <v>电导测试分液瓶数</v>
-      </c>
-      <c r="J1" t="str">
-        <v>LiFSI(g)</v>
-      </c>
-      <c r="K1" t="str">
-        <v>LiDFOB(g)</v>
-      </c>
-      <c r="L1" t="str">
-        <v>DTD(g)</v>
-      </c>
-      <c r="M1" t="str">
-        <v>SA(g)</v>
-      </c>
-      <c r="N1" t="str">
-        <v>LiNO3(g)</v>
-      </c>
-      <c r="O1" t="str">
-        <v>LiPO2F2(g)</v>
-      </c>
-      <c r="P1" t="str">
-        <v>EC(g)</v>
-      </c>
-      <c r="Q1" t="str">
-        <v>VC(g)</v>
-      </c>
-      <c r="R1" t="str">
-        <v>AND(g)</v>
-      </c>
-      <c r="S1" t="str">
-        <v>HTCN(g)</v>
-      </c>
-      <c r="T1" t="str">
-        <v>DENE(g)</v>
-      </c>
-      <c r="U1" t="str">
-        <v>TMSP(g)</v>
-      </c>
-      <c r="V1" t="str">
-        <v>TMSB(g)</v>
-      </c>
-      <c r="W1" t="str">
-        <v>EP(g)</v>
-      </c>
-      <c r="X1" t="str">
-        <v>DEC(g)</v>
-      </c>
-      <c r="Y1" t="str">
-        <v>EMC(g)</v>
-      </c>
-      <c r="Z1" t="str">
-        <v>SN(g)</v>
-      </c>
-      <c r="AA1" t="str">
-        <v>DMC(g)</v>
-      </c>
-      <c r="AB1" t="str">
-        <v>FEC(g)</v>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>TEST-02</v>
-      </c>
-      <c r="B2" t="str">
-        <v>DP20250927001</v>
-      </c>
-      <c r="C2" t="str">
-        <v>9/27/25</v>
-      </c>
-      <c r="D2" t="str">
-        <v>配液小瓶</v>
-      </c>
-      <c r="E2" t="str">
-        <v>10</v>
-      </c>
-      <c r="F2" t="str">
-        <v>1</v>
-      </c>
-      <c r="H2" t="str">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA2">
         <v>0</v>
       </c>
-      <c r="I2" t="str">
-        <v>0</v>
-      </c>
-      <c r="J2" t="str">
-        <v>0.2</v>
-      </c>
-      <c r="K2" t="str">
-        <v>0</v>
-      </c>
-      <c r="O2" t="str">
-        <v>0</v>
-      </c>
-      <c r="P2" t="str">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="str">
-        <v>0</v>
-      </c>
-      <c r="R2" t="str">
-        <v>0</v>
-      </c>
-      <c r="S2" t="str">
-        <v>0</v>
-      </c>
-      <c r="T2" t="str">
-        <v>0</v>
-      </c>
-      <c r="U2" t="str">
-        <v>0</v>
-      </c>
-      <c r="V2" t="str">
-        <v>0</v>
-      </c>
-      <c r="W2" t="str">
-        <v>0</v>
-      </c>
-      <c r="X2" t="str">
-        <v>0</v>
-      </c>
-      <c r="Z2" t="str">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="str">
-        <v>3</v>
-      </c>
-      <c r="AB2" t="str">
-        <v>0</v>
+      <c r="AB2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AB2"/>
+    <ignoredError sqref="A2:J2 L2:Q2 A1:I1 AB2 S2:Z2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>